<commit_message>
004: fix mvn job
</commit_message>
<xml_diff>
--- a/report_3.xlsx
+++ b/report_3.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -38,22 +38,19 @@
     <t>Quantité</t>
   </si>
   <si>
-    <t>shopping with Bernini</t>
+    <t>shopping with Rubens</t>
   </si>
   <si>
-    <t>1997-03-02</t>
+    <t>1988-05-24</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Practical Granite Pants</t>
+    <t>Practical Steel Clock</t>
   </si>
   <si>
-    <t>Chicken</t>
-  </si>
-  <si>
-    <t>4.0</t>
+    <t>Blackberries</t>
   </si>
   <si>
     <t>5.0</t>
@@ -180,7 +177,7 @@
         <v>13</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[000-bug]: fix get current budget
</commit_message>
<xml_diff>
--- a/report_3.xlsx
+++ b/report_3.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -38,19 +38,22 @@
     <t>Quantité</t>
   </si>
   <si>
-    <t>shopping with Escher</t>
+    <t>shopping with Botticelli</t>
   </si>
   <si>
-    <t>2003-02-05</t>
+    <t>1983-05-02</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Durable Aluminum Pants</t>
+    <t>Intelligent Wool Chair</t>
   </si>
   <si>
-    <t>Pandanus leaves</t>
+    <t>Iceberg lettuce</t>
+  </si>
+  <si>
+    <t>2.0</t>
   </si>
   <si>
     <t>4.0</t>
@@ -177,7 +180,7 @@
         <v>13</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add update quantity feature
</commit_message>
<xml_diff>
--- a/report_3.xlsx
+++ b/report_3.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Name</t>
   </si>
@@ -38,22 +38,19 @@
     <t>Quantité</t>
   </si>
   <si>
-    <t>shopping with Manet</t>
+    <t>shopping with Diego Rivera</t>
   </si>
   <si>
-    <t>1987-09-20</t>
+    <t>1975-07-11</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Awesome Concrete Shoes</t>
+    <t>Small Copper Bench</t>
   </si>
   <si>
-    <t>Common Cultivated Mushrooms</t>
-  </si>
-  <si>
-    <t>1.0</t>
+    <t>Mung Beans</t>
   </si>
   <si>
     <t>4.0</t>
@@ -180,7 +177,7 @@
         <v>13</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>